<commit_message>
fix: methylation dict needs categories tab
</commit_message>
<xml_diff>
--- a/dictionaries/methylation_clocks/methylation_clocks-non_rep.xlsx
+++ b/dictionaries/methylation_clocks/methylation_clocks-non_rep.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sido/VisualStudioCodeProjects/ds-beta-dictionaries/dictionaries/methylation_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sido/VisualStudioCodeProjects/ds-beta-dictionaries/dictionaries/methylation_clocks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ABBB896-A61D-AE40-A05B-D18DB3D5AA50}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78E5B010-D735-4B4E-8092-353A1297DB55}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8500" yWindow="1020" windowWidth="15960" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8500" yWindow="460" windowWidth="15960" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
+    <sheet name="Categories" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
 </workbook>
@@ -1317,7 +1318,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:IP8"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -1693,4 +1694,16 @@
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CF86731-4DF2-0146-B08C-62CAF97A71CB}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feat: added age variable to include multiple timepoints
</commit_message>
<xml_diff>
--- a/dictionaries/methylation_clocks/methylation_clocks-non_rep.xlsx
+++ b/dictionaries/methylation_clocks/methylation_clocks-non_rep.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sido/VisualStudioCodeProjects/ds-beta-dictionaries/dictionaries/methylation_clocks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78E5B010-D735-4B4E-8092-353A1297DB55}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBBBDD71-02A7-3A41-97DA-F540ABABD488}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8500" yWindow="460" windowWidth="15960" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8500" yWindow="460" windowWidth="15960" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
   <si>
     <t>name</t>
   </si>
@@ -78,6 +78,15 @@
   </si>
   <si>
     <t>BNN measure</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>Age when the clocks where measured</t>
   </si>
 </sst>
 </file>
@@ -1316,16 +1325,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:IP8"/>
+  <dimension ref="A1:IP9"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="3" width="8.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="25.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="250" width="8.83203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1605,35 +1614,281 @@
     </row>
     <row r="3" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>10</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
+      <c r="R3" s="4"/>
+      <c r="S3" s="4"/>
+      <c r="T3" s="4"/>
+      <c r="U3" s="4"/>
+      <c r="V3" s="4"/>
+      <c r="W3" s="4"/>
+      <c r="X3" s="4"/>
+      <c r="Y3" s="4"/>
+      <c r="Z3" s="4"/>
+      <c r="AA3" s="4"/>
+      <c r="AB3" s="4"/>
+      <c r="AC3" s="4"/>
+      <c r="AD3" s="4"/>
+      <c r="AE3" s="4"/>
+      <c r="AF3" s="4"/>
+      <c r="AG3" s="4"/>
+      <c r="AH3" s="4"/>
+      <c r="AI3" s="4"/>
+      <c r="AJ3" s="4"/>
+      <c r="AK3" s="4"/>
+      <c r="AL3" s="4"/>
+      <c r="AM3" s="4"/>
+      <c r="AN3" s="4"/>
+      <c r="AO3" s="4"/>
+      <c r="AP3" s="4"/>
+      <c r="AQ3" s="4"/>
+      <c r="AR3" s="4"/>
+      <c r="AS3" s="4"/>
+      <c r="AT3" s="4"/>
+      <c r="AU3" s="4"/>
+      <c r="AV3" s="4"/>
+      <c r="AW3" s="4"/>
+      <c r="AX3" s="4"/>
+      <c r="AY3" s="4"/>
+      <c r="AZ3" s="4"/>
+      <c r="BA3" s="4"/>
+      <c r="BB3" s="4"/>
+      <c r="BC3" s="4"/>
+      <c r="BD3" s="4"/>
+      <c r="BE3" s="4"/>
+      <c r="BF3" s="4"/>
+      <c r="BG3" s="4"/>
+      <c r="BH3" s="4"/>
+      <c r="BI3" s="4"/>
+      <c r="BJ3" s="4"/>
+      <c r="BK3" s="4"/>
+      <c r="BL3" s="4"/>
+      <c r="BM3" s="4"/>
+      <c r="BN3" s="4"/>
+      <c r="BO3" s="4"/>
+      <c r="BP3" s="4"/>
+      <c r="BQ3" s="4"/>
+      <c r="BR3" s="4"/>
+      <c r="BS3" s="4"/>
+      <c r="BT3" s="4"/>
+      <c r="BU3" s="4"/>
+      <c r="BV3" s="4"/>
+      <c r="BW3" s="4"/>
+      <c r="BX3" s="4"/>
+      <c r="BY3" s="4"/>
+      <c r="BZ3" s="4"/>
+      <c r="CA3" s="4"/>
+      <c r="CB3" s="4"/>
+      <c r="CC3" s="4"/>
+      <c r="CD3" s="4"/>
+      <c r="CE3" s="4"/>
+      <c r="CF3" s="4"/>
+      <c r="CG3" s="4"/>
+      <c r="CH3" s="4"/>
+      <c r="CI3" s="4"/>
+      <c r="CJ3" s="4"/>
+      <c r="CK3" s="4"/>
+      <c r="CL3" s="4"/>
+      <c r="CM3" s="4"/>
+      <c r="CN3" s="4"/>
+      <c r="CO3" s="4"/>
+      <c r="CP3" s="4"/>
+      <c r="CQ3" s="4"/>
+      <c r="CR3" s="4"/>
+      <c r="CS3" s="4"/>
+      <c r="CT3" s="4"/>
+      <c r="CU3" s="4"/>
+      <c r="CV3" s="4"/>
+      <c r="CW3" s="4"/>
+      <c r="CX3" s="4"/>
+      <c r="CY3" s="4"/>
+      <c r="CZ3" s="4"/>
+      <c r="DA3" s="4"/>
+      <c r="DB3" s="4"/>
+      <c r="DC3" s="4"/>
+      <c r="DD3" s="4"/>
+      <c r="DE3" s="4"/>
+      <c r="DF3" s="4"/>
+      <c r="DG3" s="4"/>
+      <c r="DH3" s="4"/>
+      <c r="DI3" s="4"/>
+      <c r="DJ3" s="4"/>
+      <c r="DK3" s="4"/>
+      <c r="DL3" s="4"/>
+      <c r="DM3" s="4"/>
+      <c r="DN3" s="4"/>
+      <c r="DO3" s="4"/>
+      <c r="DP3" s="4"/>
+      <c r="DQ3" s="4"/>
+      <c r="DR3" s="4"/>
+      <c r="DS3" s="4"/>
+      <c r="DT3" s="4"/>
+      <c r="DU3" s="4"/>
+      <c r="DV3" s="4"/>
+      <c r="DW3" s="4"/>
+      <c r="DX3" s="4"/>
+      <c r="DY3" s="4"/>
+      <c r="DZ3" s="4"/>
+      <c r="EA3" s="4"/>
+      <c r="EB3" s="4"/>
+      <c r="EC3" s="4"/>
+      <c r="ED3" s="4"/>
+      <c r="EE3" s="4"/>
+      <c r="EF3" s="4"/>
+      <c r="EG3" s="4"/>
+      <c r="EH3" s="4"/>
+      <c r="EI3" s="4"/>
+      <c r="EJ3" s="4"/>
+      <c r="EK3" s="4"/>
+      <c r="EL3" s="4"/>
+      <c r="EM3" s="4"/>
+      <c r="EN3" s="4"/>
+      <c r="EO3" s="4"/>
+      <c r="EP3" s="4"/>
+      <c r="EQ3" s="4"/>
+      <c r="ER3" s="4"/>
+      <c r="ES3" s="4"/>
+      <c r="ET3" s="4"/>
+      <c r="EU3" s="4"/>
+      <c r="EV3" s="4"/>
+      <c r="EW3" s="4"/>
+      <c r="EX3" s="4"/>
+      <c r="EY3" s="4"/>
+      <c r="EZ3" s="4"/>
+      <c r="FA3" s="4"/>
+      <c r="FB3" s="4"/>
+      <c r="FC3" s="4"/>
+      <c r="FD3" s="4"/>
+      <c r="FE3" s="4"/>
+      <c r="FF3" s="4"/>
+      <c r="FG3" s="4"/>
+      <c r="FH3" s="4"/>
+      <c r="FI3" s="4"/>
+      <c r="FJ3" s="4"/>
+      <c r="FK3" s="4"/>
+      <c r="FL3" s="4"/>
+      <c r="FM3" s="4"/>
+      <c r="FN3" s="4"/>
+      <c r="FO3" s="4"/>
+      <c r="FP3" s="4"/>
+      <c r="FQ3" s="4"/>
+      <c r="FR3" s="4"/>
+      <c r="FS3" s="4"/>
+      <c r="FT3" s="4"/>
+      <c r="FU3" s="4"/>
+      <c r="FV3" s="4"/>
+      <c r="FW3" s="4"/>
+      <c r="FX3" s="4"/>
+      <c r="FY3" s="4"/>
+      <c r="FZ3" s="4"/>
+      <c r="GA3" s="4"/>
+      <c r="GB3" s="4"/>
+      <c r="GC3" s="4"/>
+      <c r="GD3" s="4"/>
+      <c r="GE3" s="4"/>
+      <c r="GF3" s="4"/>
+      <c r="GG3" s="4"/>
+      <c r="GH3" s="4"/>
+      <c r="GI3" s="4"/>
+      <c r="GJ3" s="4"/>
+      <c r="GK3" s="4"/>
+      <c r="GL3" s="4"/>
+      <c r="GM3" s="4"/>
+      <c r="GN3" s="4"/>
+      <c r="GO3" s="4"/>
+      <c r="GP3" s="4"/>
+      <c r="GQ3" s="4"/>
+      <c r="GR3" s="4"/>
+      <c r="GS3" s="4"/>
+      <c r="GT3" s="4"/>
+      <c r="GU3" s="4"/>
+      <c r="GV3" s="4"/>
+      <c r="GW3" s="4"/>
+      <c r="GX3" s="4"/>
+      <c r="GY3" s="4"/>
+      <c r="GZ3" s="4"/>
+      <c r="HA3" s="4"/>
+      <c r="HB3" s="4"/>
+      <c r="HC3" s="4"/>
+      <c r="HD3" s="4"/>
+      <c r="HE3" s="4"/>
+      <c r="HF3" s="4"/>
+      <c r="HG3" s="4"/>
+      <c r="HH3" s="4"/>
+      <c r="HI3" s="4"/>
+      <c r="HJ3" s="4"/>
+      <c r="HK3" s="4"/>
+      <c r="HL3" s="4"/>
+      <c r="HM3" s="4"/>
+      <c r="HN3" s="4"/>
+      <c r="HO3" s="4"/>
+      <c r="HP3" s="4"/>
+      <c r="HQ3" s="4"/>
+      <c r="HR3" s="4"/>
+      <c r="HS3" s="4"/>
+      <c r="HT3" s="4"/>
+      <c r="HU3" s="4"/>
+      <c r="HV3" s="4"/>
+      <c r="HW3" s="4"/>
+      <c r="HX3" s="4"/>
+      <c r="HY3" s="4"/>
+      <c r="HZ3" s="4"/>
+      <c r="IA3" s="4"/>
+      <c r="IB3" s="4"/>
+      <c r="IC3" s="4"/>
+      <c r="ID3" s="4"/>
+      <c r="IE3" s="4"/>
+      <c r="IF3" s="4"/>
+      <c r="IG3" s="4"/>
+      <c r="IH3" s="4"/>
+      <c r="II3" s="4"/>
+      <c r="IJ3" s="4"/>
+      <c r="IK3" s="4"/>
+      <c r="IL3" s="4"/>
+      <c r="IM3" s="4"/>
+      <c r="IN3" s="4"/>
+      <c r="IO3" s="4"/>
+      <c r="IP3" s="4"/>
     </row>
     <row r="4" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="3" t="s">
+      <c r="A4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>11</v>
+      <c r="D4" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>13</v>
+      <c r="A5" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>9</v>
@@ -1641,13 +1896,13 @@
       <c r="C5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>17</v>
+      <c r="D5" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>9</v>
@@ -1656,12 +1911,12 @@
         <v>5</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>9</v>
@@ -1670,12 +1925,12 @@
         <v>5</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>9</v>
@@ -1684,6 +1939,20 @@
         <v>5</v>
       </c>
       <c r="D8" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1700,7 +1969,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CF86731-4DF2-0146-B08C-62CAF97A71CB}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>

</xml_diff>

<commit_message>
feat: added row_id to methyl dict
</commit_message>
<xml_diff>
--- a/dictionaries/methylation_clocks/methylation_clocks-non_rep.xlsx
+++ b/dictionaries/methylation_clocks/methylation_clocks-non_rep.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sido/VisualStudioCodeProjects/ds-beta-dictionaries/dictionaries/methylation_clocks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBBBDD71-02A7-3A41-97DA-F540ABABD488}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD263E1F-3BD5-BC46-87CF-A4C5E73C5B3E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8500" yWindow="460" windowWidth="15960" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="24">
   <si>
     <t>name</t>
   </si>
@@ -87,6 +87,12 @@
   </si>
   <si>
     <t>Age when the clocks where measured</t>
+  </si>
+  <si>
+    <t>row_id</t>
+  </si>
+  <si>
+    <t>Identifier for Opal</t>
   </si>
 </sst>
 </file>
@@ -1325,10 +1331,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:IP9"/>
+  <dimension ref="A1:IP10"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1354,16 +1360,16 @@
     </row>
     <row r="2" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
@@ -1614,16 +1620,16 @@
     </row>
     <row r="3" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
@@ -1874,35 +1880,281 @@
     </row>
     <row r="4" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>10</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="4"/>
+      <c r="T4" s="4"/>
+      <c r="U4" s="4"/>
+      <c r="V4" s="4"/>
+      <c r="W4" s="4"/>
+      <c r="X4" s="4"/>
+      <c r="Y4" s="4"/>
+      <c r="Z4" s="4"/>
+      <c r="AA4" s="4"/>
+      <c r="AB4" s="4"/>
+      <c r="AC4" s="4"/>
+      <c r="AD4" s="4"/>
+      <c r="AE4" s="4"/>
+      <c r="AF4" s="4"/>
+      <c r="AG4" s="4"/>
+      <c r="AH4" s="4"/>
+      <c r="AI4" s="4"/>
+      <c r="AJ4" s="4"/>
+      <c r="AK4" s="4"/>
+      <c r="AL4" s="4"/>
+      <c r="AM4" s="4"/>
+      <c r="AN4" s="4"/>
+      <c r="AO4" s="4"/>
+      <c r="AP4" s="4"/>
+      <c r="AQ4" s="4"/>
+      <c r="AR4" s="4"/>
+      <c r="AS4" s="4"/>
+      <c r="AT4" s="4"/>
+      <c r="AU4" s="4"/>
+      <c r="AV4" s="4"/>
+      <c r="AW4" s="4"/>
+      <c r="AX4" s="4"/>
+      <c r="AY4" s="4"/>
+      <c r="AZ4" s="4"/>
+      <c r="BA4" s="4"/>
+      <c r="BB4" s="4"/>
+      <c r="BC4" s="4"/>
+      <c r="BD4" s="4"/>
+      <c r="BE4" s="4"/>
+      <c r="BF4" s="4"/>
+      <c r="BG4" s="4"/>
+      <c r="BH4" s="4"/>
+      <c r="BI4" s="4"/>
+      <c r="BJ4" s="4"/>
+      <c r="BK4" s="4"/>
+      <c r="BL4" s="4"/>
+      <c r="BM4" s="4"/>
+      <c r="BN4" s="4"/>
+      <c r="BO4" s="4"/>
+      <c r="BP4" s="4"/>
+      <c r="BQ4" s="4"/>
+      <c r="BR4" s="4"/>
+      <c r="BS4" s="4"/>
+      <c r="BT4" s="4"/>
+      <c r="BU4" s="4"/>
+      <c r="BV4" s="4"/>
+      <c r="BW4" s="4"/>
+      <c r="BX4" s="4"/>
+      <c r="BY4" s="4"/>
+      <c r="BZ4" s="4"/>
+      <c r="CA4" s="4"/>
+      <c r="CB4" s="4"/>
+      <c r="CC4" s="4"/>
+      <c r="CD4" s="4"/>
+      <c r="CE4" s="4"/>
+      <c r="CF4" s="4"/>
+      <c r="CG4" s="4"/>
+      <c r="CH4" s="4"/>
+      <c r="CI4" s="4"/>
+      <c r="CJ4" s="4"/>
+      <c r="CK4" s="4"/>
+      <c r="CL4" s="4"/>
+      <c r="CM4" s="4"/>
+      <c r="CN4" s="4"/>
+      <c r="CO4" s="4"/>
+      <c r="CP4" s="4"/>
+      <c r="CQ4" s="4"/>
+      <c r="CR4" s="4"/>
+      <c r="CS4" s="4"/>
+      <c r="CT4" s="4"/>
+      <c r="CU4" s="4"/>
+      <c r="CV4" s="4"/>
+      <c r="CW4" s="4"/>
+      <c r="CX4" s="4"/>
+      <c r="CY4" s="4"/>
+      <c r="CZ4" s="4"/>
+      <c r="DA4" s="4"/>
+      <c r="DB4" s="4"/>
+      <c r="DC4" s="4"/>
+      <c r="DD4" s="4"/>
+      <c r="DE4" s="4"/>
+      <c r="DF4" s="4"/>
+      <c r="DG4" s="4"/>
+      <c r="DH4" s="4"/>
+      <c r="DI4" s="4"/>
+      <c r="DJ4" s="4"/>
+      <c r="DK4" s="4"/>
+      <c r="DL4" s="4"/>
+      <c r="DM4" s="4"/>
+      <c r="DN4" s="4"/>
+      <c r="DO4" s="4"/>
+      <c r="DP4" s="4"/>
+      <c r="DQ4" s="4"/>
+      <c r="DR4" s="4"/>
+      <c r="DS4" s="4"/>
+      <c r="DT4" s="4"/>
+      <c r="DU4" s="4"/>
+      <c r="DV4" s="4"/>
+      <c r="DW4" s="4"/>
+      <c r="DX4" s="4"/>
+      <c r="DY4" s="4"/>
+      <c r="DZ4" s="4"/>
+      <c r="EA4" s="4"/>
+      <c r="EB4" s="4"/>
+      <c r="EC4" s="4"/>
+      <c r="ED4" s="4"/>
+      <c r="EE4" s="4"/>
+      <c r="EF4" s="4"/>
+      <c r="EG4" s="4"/>
+      <c r="EH4" s="4"/>
+      <c r="EI4" s="4"/>
+      <c r="EJ4" s="4"/>
+      <c r="EK4" s="4"/>
+      <c r="EL4" s="4"/>
+      <c r="EM4" s="4"/>
+      <c r="EN4" s="4"/>
+      <c r="EO4" s="4"/>
+      <c r="EP4" s="4"/>
+      <c r="EQ4" s="4"/>
+      <c r="ER4" s="4"/>
+      <c r="ES4" s="4"/>
+      <c r="ET4" s="4"/>
+      <c r="EU4" s="4"/>
+      <c r="EV4" s="4"/>
+      <c r="EW4" s="4"/>
+      <c r="EX4" s="4"/>
+      <c r="EY4" s="4"/>
+      <c r="EZ4" s="4"/>
+      <c r="FA4" s="4"/>
+      <c r="FB4" s="4"/>
+      <c r="FC4" s="4"/>
+      <c r="FD4" s="4"/>
+      <c r="FE4" s="4"/>
+      <c r="FF4" s="4"/>
+      <c r="FG4" s="4"/>
+      <c r="FH4" s="4"/>
+      <c r="FI4" s="4"/>
+      <c r="FJ4" s="4"/>
+      <c r="FK4" s="4"/>
+      <c r="FL4" s="4"/>
+      <c r="FM4" s="4"/>
+      <c r="FN4" s="4"/>
+      <c r="FO4" s="4"/>
+      <c r="FP4" s="4"/>
+      <c r="FQ4" s="4"/>
+      <c r="FR4" s="4"/>
+      <c r="FS4" s="4"/>
+      <c r="FT4" s="4"/>
+      <c r="FU4" s="4"/>
+      <c r="FV4" s="4"/>
+      <c r="FW4" s="4"/>
+      <c r="FX4" s="4"/>
+      <c r="FY4" s="4"/>
+      <c r="FZ4" s="4"/>
+      <c r="GA4" s="4"/>
+      <c r="GB4" s="4"/>
+      <c r="GC4" s="4"/>
+      <c r="GD4" s="4"/>
+      <c r="GE4" s="4"/>
+      <c r="GF4" s="4"/>
+      <c r="GG4" s="4"/>
+      <c r="GH4" s="4"/>
+      <c r="GI4" s="4"/>
+      <c r="GJ4" s="4"/>
+      <c r="GK4" s="4"/>
+      <c r="GL4" s="4"/>
+      <c r="GM4" s="4"/>
+      <c r="GN4" s="4"/>
+      <c r="GO4" s="4"/>
+      <c r="GP4" s="4"/>
+      <c r="GQ4" s="4"/>
+      <c r="GR4" s="4"/>
+      <c r="GS4" s="4"/>
+      <c r="GT4" s="4"/>
+      <c r="GU4" s="4"/>
+      <c r="GV4" s="4"/>
+      <c r="GW4" s="4"/>
+      <c r="GX4" s="4"/>
+      <c r="GY4" s="4"/>
+      <c r="GZ4" s="4"/>
+      <c r="HA4" s="4"/>
+      <c r="HB4" s="4"/>
+      <c r="HC4" s="4"/>
+      <c r="HD4" s="4"/>
+      <c r="HE4" s="4"/>
+      <c r="HF4" s="4"/>
+      <c r="HG4" s="4"/>
+      <c r="HH4" s="4"/>
+      <c r="HI4" s="4"/>
+      <c r="HJ4" s="4"/>
+      <c r="HK4" s="4"/>
+      <c r="HL4" s="4"/>
+      <c r="HM4" s="4"/>
+      <c r="HN4" s="4"/>
+      <c r="HO4" s="4"/>
+      <c r="HP4" s="4"/>
+      <c r="HQ4" s="4"/>
+      <c r="HR4" s="4"/>
+      <c r="HS4" s="4"/>
+      <c r="HT4" s="4"/>
+      <c r="HU4" s="4"/>
+      <c r="HV4" s="4"/>
+      <c r="HW4" s="4"/>
+      <c r="HX4" s="4"/>
+      <c r="HY4" s="4"/>
+      <c r="HZ4" s="4"/>
+      <c r="IA4" s="4"/>
+      <c r="IB4" s="4"/>
+      <c r="IC4" s="4"/>
+      <c r="ID4" s="4"/>
+      <c r="IE4" s="4"/>
+      <c r="IF4" s="4"/>
+      <c r="IG4" s="4"/>
+      <c r="IH4" s="4"/>
+      <c r="II4" s="4"/>
+      <c r="IJ4" s="4"/>
+      <c r="IK4" s="4"/>
+      <c r="IL4" s="4"/>
+      <c r="IM4" s="4"/>
+      <c r="IN4" s="4"/>
+      <c r="IO4" s="4"/>
+      <c r="IP4" s="4"/>
     </row>
     <row r="5" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="3" t="s">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>11</v>
+      <c r="D5" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>13</v>
+      <c r="A6" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>9</v>
@@ -1910,13 +2162,13 @@
       <c r="C6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>17</v>
+      <c r="D6" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>9</v>
@@ -1925,12 +2177,12 @@
         <v>5</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>9</v>
@@ -1939,12 +2191,12 @@
         <v>5</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>9</v>
@@ -1953,6 +2205,20 @@
         <v>5</v>
       </c>
       <c r="D9" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: removed the row_id again
</commit_message>
<xml_diff>
--- a/dictionaries/methylation_clocks/methylation_clocks-non_rep.xlsx
+++ b/dictionaries/methylation_clocks/methylation_clocks-non_rep.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sido/VisualStudioCodeProjects/ds-beta-dictionaries/dictionaries/methylation_clocks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD263E1F-3BD5-BC46-87CF-A4C5E73C5B3E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB2C356B-1B03-8C48-882E-A081F5BA33D3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8500" yWindow="460" windowWidth="15960" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
   <si>
     <t>name</t>
   </si>
@@ -87,12 +87,6 @@
   </si>
   <si>
     <t>Age when the clocks where measured</t>
-  </si>
-  <si>
-    <t>row_id</t>
-  </si>
-  <si>
-    <t>Identifier for Opal</t>
   </si>
 </sst>
 </file>
@@ -1331,10 +1325,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:IP10"/>
+  <dimension ref="A1:IP9"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1360,16 +1354,16 @@
     </row>
     <row r="2" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
@@ -1620,16 +1614,16 @@
     </row>
     <row r="3" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
@@ -1880,281 +1874,35 @@
     </row>
     <row r="4" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-      <c r="P4" s="4"/>
-      <c r="Q4" s="4"/>
-      <c r="R4" s="4"/>
-      <c r="S4" s="4"/>
-      <c r="T4" s="4"/>
-      <c r="U4" s="4"/>
-      <c r="V4" s="4"/>
-      <c r="W4" s="4"/>
-      <c r="X4" s="4"/>
-      <c r="Y4" s="4"/>
-      <c r="Z4" s="4"/>
-      <c r="AA4" s="4"/>
-      <c r="AB4" s="4"/>
-      <c r="AC4" s="4"/>
-      <c r="AD4" s="4"/>
-      <c r="AE4" s="4"/>
-      <c r="AF4" s="4"/>
-      <c r="AG4" s="4"/>
-      <c r="AH4" s="4"/>
-      <c r="AI4" s="4"/>
-      <c r="AJ4" s="4"/>
-      <c r="AK4" s="4"/>
-      <c r="AL4" s="4"/>
-      <c r="AM4" s="4"/>
-      <c r="AN4" s="4"/>
-      <c r="AO4" s="4"/>
-      <c r="AP4" s="4"/>
-      <c r="AQ4" s="4"/>
-      <c r="AR4" s="4"/>
-      <c r="AS4" s="4"/>
-      <c r="AT4" s="4"/>
-      <c r="AU4" s="4"/>
-      <c r="AV4" s="4"/>
-      <c r="AW4" s="4"/>
-      <c r="AX4" s="4"/>
-      <c r="AY4" s="4"/>
-      <c r="AZ4" s="4"/>
-      <c r="BA4" s="4"/>
-      <c r="BB4" s="4"/>
-      <c r="BC4" s="4"/>
-      <c r="BD4" s="4"/>
-      <c r="BE4" s="4"/>
-      <c r="BF4" s="4"/>
-      <c r="BG4" s="4"/>
-      <c r="BH4" s="4"/>
-      <c r="BI4" s="4"/>
-      <c r="BJ4" s="4"/>
-      <c r="BK4" s="4"/>
-      <c r="BL4" s="4"/>
-      <c r="BM4" s="4"/>
-      <c r="BN4" s="4"/>
-      <c r="BO4" s="4"/>
-      <c r="BP4" s="4"/>
-      <c r="BQ4" s="4"/>
-      <c r="BR4" s="4"/>
-      <c r="BS4" s="4"/>
-      <c r="BT4" s="4"/>
-      <c r="BU4" s="4"/>
-      <c r="BV4" s="4"/>
-      <c r="BW4" s="4"/>
-      <c r="BX4" s="4"/>
-      <c r="BY4" s="4"/>
-      <c r="BZ4" s="4"/>
-      <c r="CA4" s="4"/>
-      <c r="CB4" s="4"/>
-      <c r="CC4" s="4"/>
-      <c r="CD4" s="4"/>
-      <c r="CE4" s="4"/>
-      <c r="CF4" s="4"/>
-      <c r="CG4" s="4"/>
-      <c r="CH4" s="4"/>
-      <c r="CI4" s="4"/>
-      <c r="CJ4" s="4"/>
-      <c r="CK4" s="4"/>
-      <c r="CL4" s="4"/>
-      <c r="CM4" s="4"/>
-      <c r="CN4" s="4"/>
-      <c r="CO4" s="4"/>
-      <c r="CP4" s="4"/>
-      <c r="CQ4" s="4"/>
-      <c r="CR4" s="4"/>
-      <c r="CS4" s="4"/>
-      <c r="CT4" s="4"/>
-      <c r="CU4" s="4"/>
-      <c r="CV4" s="4"/>
-      <c r="CW4" s="4"/>
-      <c r="CX4" s="4"/>
-      <c r="CY4" s="4"/>
-      <c r="CZ4" s="4"/>
-      <c r="DA4" s="4"/>
-      <c r="DB4" s="4"/>
-      <c r="DC4" s="4"/>
-      <c r="DD4" s="4"/>
-      <c r="DE4" s="4"/>
-      <c r="DF4" s="4"/>
-      <c r="DG4" s="4"/>
-      <c r="DH4" s="4"/>
-      <c r="DI4" s="4"/>
-      <c r="DJ4" s="4"/>
-      <c r="DK4" s="4"/>
-      <c r="DL4" s="4"/>
-      <c r="DM4" s="4"/>
-      <c r="DN4" s="4"/>
-      <c r="DO4" s="4"/>
-      <c r="DP4" s="4"/>
-      <c r="DQ4" s="4"/>
-      <c r="DR4" s="4"/>
-      <c r="DS4" s="4"/>
-      <c r="DT4" s="4"/>
-      <c r="DU4" s="4"/>
-      <c r="DV4" s="4"/>
-      <c r="DW4" s="4"/>
-      <c r="DX4" s="4"/>
-      <c r="DY4" s="4"/>
-      <c r="DZ4" s="4"/>
-      <c r="EA4" s="4"/>
-      <c r="EB4" s="4"/>
-      <c r="EC4" s="4"/>
-      <c r="ED4" s="4"/>
-      <c r="EE4" s="4"/>
-      <c r="EF4" s="4"/>
-      <c r="EG4" s="4"/>
-      <c r="EH4" s="4"/>
-      <c r="EI4" s="4"/>
-      <c r="EJ4" s="4"/>
-      <c r="EK4" s="4"/>
-      <c r="EL4" s="4"/>
-      <c r="EM4" s="4"/>
-      <c r="EN4" s="4"/>
-      <c r="EO4" s="4"/>
-      <c r="EP4" s="4"/>
-      <c r="EQ4" s="4"/>
-      <c r="ER4" s="4"/>
-      <c r="ES4" s="4"/>
-      <c r="ET4" s="4"/>
-      <c r="EU4" s="4"/>
-      <c r="EV4" s="4"/>
-      <c r="EW4" s="4"/>
-      <c r="EX4" s="4"/>
-      <c r="EY4" s="4"/>
-      <c r="EZ4" s="4"/>
-      <c r="FA4" s="4"/>
-      <c r="FB4" s="4"/>
-      <c r="FC4" s="4"/>
-      <c r="FD4" s="4"/>
-      <c r="FE4" s="4"/>
-      <c r="FF4" s="4"/>
-      <c r="FG4" s="4"/>
-      <c r="FH4" s="4"/>
-      <c r="FI4" s="4"/>
-      <c r="FJ4" s="4"/>
-      <c r="FK4" s="4"/>
-      <c r="FL4" s="4"/>
-      <c r="FM4" s="4"/>
-      <c r="FN4" s="4"/>
-      <c r="FO4" s="4"/>
-      <c r="FP4" s="4"/>
-      <c r="FQ4" s="4"/>
-      <c r="FR4" s="4"/>
-      <c r="FS4" s="4"/>
-      <c r="FT4" s="4"/>
-      <c r="FU4" s="4"/>
-      <c r="FV4" s="4"/>
-      <c r="FW4" s="4"/>
-      <c r="FX4" s="4"/>
-      <c r="FY4" s="4"/>
-      <c r="FZ4" s="4"/>
-      <c r="GA4" s="4"/>
-      <c r="GB4" s="4"/>
-      <c r="GC4" s="4"/>
-      <c r="GD4" s="4"/>
-      <c r="GE4" s="4"/>
-      <c r="GF4" s="4"/>
-      <c r="GG4" s="4"/>
-      <c r="GH4" s="4"/>
-      <c r="GI4" s="4"/>
-      <c r="GJ4" s="4"/>
-      <c r="GK4" s="4"/>
-      <c r="GL4" s="4"/>
-      <c r="GM4" s="4"/>
-      <c r="GN4" s="4"/>
-      <c r="GO4" s="4"/>
-      <c r="GP4" s="4"/>
-      <c r="GQ4" s="4"/>
-      <c r="GR4" s="4"/>
-      <c r="GS4" s="4"/>
-      <c r="GT4" s="4"/>
-      <c r="GU4" s="4"/>
-      <c r="GV4" s="4"/>
-      <c r="GW4" s="4"/>
-      <c r="GX4" s="4"/>
-      <c r="GY4" s="4"/>
-      <c r="GZ4" s="4"/>
-      <c r="HA4" s="4"/>
-      <c r="HB4" s="4"/>
-      <c r="HC4" s="4"/>
-      <c r="HD4" s="4"/>
-      <c r="HE4" s="4"/>
-      <c r="HF4" s="4"/>
-      <c r="HG4" s="4"/>
-      <c r="HH4" s="4"/>
-      <c r="HI4" s="4"/>
-      <c r="HJ4" s="4"/>
-      <c r="HK4" s="4"/>
-      <c r="HL4" s="4"/>
-      <c r="HM4" s="4"/>
-      <c r="HN4" s="4"/>
-      <c r="HO4" s="4"/>
-      <c r="HP4" s="4"/>
-      <c r="HQ4" s="4"/>
-      <c r="HR4" s="4"/>
-      <c r="HS4" s="4"/>
-      <c r="HT4" s="4"/>
-      <c r="HU4" s="4"/>
-      <c r="HV4" s="4"/>
-      <c r="HW4" s="4"/>
-      <c r="HX4" s="4"/>
-      <c r="HY4" s="4"/>
-      <c r="HZ4" s="4"/>
-      <c r="IA4" s="4"/>
-      <c r="IB4" s="4"/>
-      <c r="IC4" s="4"/>
-      <c r="ID4" s="4"/>
-      <c r="IE4" s="4"/>
-      <c r="IF4" s="4"/>
-      <c r="IG4" s="4"/>
-      <c r="IH4" s="4"/>
-      <c r="II4" s="4"/>
-      <c r="IJ4" s="4"/>
-      <c r="IK4" s="4"/>
-      <c r="IL4" s="4"/>
-      <c r="IM4" s="4"/>
-      <c r="IN4" s="4"/>
-      <c r="IO4" s="4"/>
-      <c r="IP4" s="4"/>
+        <v>10</v>
+      </c>
     </row>
     <row r="5" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="2" t="s">
+      <c r="A5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>10</v>
+      <c r="D5" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>12</v>
+      <c r="A6" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>9</v>
@@ -2162,13 +1910,13 @@
       <c r="C6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>11</v>
+      <c r="D6" s="5" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>9</v>
@@ -2177,12 +1925,12 @@
         <v>5</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>9</v>
@@ -2191,12 +1939,12 @@
         <v>5</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>9</v>
@@ -2205,20 +1953,6 @@
         <v>5</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="5" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>